<commit_message>
Ajout de la presence de pcmn dans les herbes
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\first_flutter_app\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23421669-C9D6-4C8B-BC84-476A74A5B8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5B55ED-44D5-4A34-B3BA-A74723665B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1365" windowWidth="27000" windowHeight="14235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
     <sheet name="element_terrain" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="pokemon" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="21">
   <si>
     <t>HERBE</t>
   </si>
@@ -60,6 +60,36 @@
   </si>
   <si>
     <t>assets/for_alex/rocher.png</t>
+  </si>
+  <si>
+    <t>% proba trouver pokemon (ex: 60)</t>
+  </si>
+  <si>
+    <t>Nom pokemon (ex: Pikatchu)</t>
+  </si>
+  <si>
+    <t>Pikachu</t>
+  </si>
+  <si>
+    <t>Mewtwo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chemin image pkmn (ex: </t>
+  </si>
+  <si>
+    <t>path_pikachu</t>
+  </si>
+  <si>
+    <t>path_mewtwo</t>
+  </si>
+  <si>
+    <t>rareté (%)</t>
+  </si>
+  <si>
+    <t>66.7</t>
+  </si>
+  <si>
+    <t>33.3</t>
   </si>
 </sst>
 </file>
@@ -386,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
@@ -1106,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D212DAE-41B9-48BB-90C6-C7B81A14720A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,7 +1191,18 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>80</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -1185,12 +1226,57 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44DE501-A4F1-4E55-9F83-CC17A103164F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout de pikachu et mewtwo dans les herbes
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\first_flutter_app\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5B55ED-44D5-4A34-B3BA-A74723665B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877B8F1E-3E8E-4249-AB91-8D3ACBB5372A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1365" windowWidth="27000" windowHeight="14235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1365" windowWidth="27000" windowHeight="14235" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
@@ -77,19 +77,19 @@
     <t xml:space="preserve">chemin image pkmn (ex: </t>
   </si>
   <si>
-    <t>path_pikachu</t>
-  </si>
-  <si>
-    <t>path_mewtwo</t>
-  </si>
-  <si>
     <t>rareté (%)</t>
   </si>
   <si>
-    <t>66.7</t>
-  </si>
-  <si>
-    <t>33.3</t>
+    <t>assets/for_alex/pikachu.png</t>
+  </si>
+  <si>
+    <t>assets/for_alex/mewtwo.png</t>
+  </si>
+  <si>
+    <t>80.0</t>
+  </si>
+  <si>
+    <t>20.0</t>
   </si>
 </sst>
 </file>
@@ -1136,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D212DAE-41B9-48BB-90C6-C7B81A14720A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,13 +1228,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44DE501-A4F1-4E55-9F83-CC17A103164F}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1253,15 +1255,15 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
lecture exel en convention verticale
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\first_flutter_app\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877B8F1E-3E8E-4249-AB91-8D3ACBB5372A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF35D9D-AE73-494D-B85D-D372A4D2604E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1365" windowWidth="27000" windowHeight="14235" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6645" yWindow="3585" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Mewtwo</t>
   </si>
   <si>
-    <t xml:space="preserve">chemin image pkmn (ex: </t>
-  </si>
-  <si>
     <t>rareté (%)</t>
   </si>
   <si>
@@ -86,10 +83,13 @@
     <t>assets/for_alex/mewtwo.png</t>
   </si>
   <si>
-    <t>80.0</t>
-  </si>
-  <si>
-    <t>20.0</t>
+    <t>chemin image pkmn (ex: /assets … )</t>
+  </si>
+  <si>
+    <t>66.7</t>
+  </si>
+  <si>
+    <t>33.3</t>
   </si>
 </sst>
 </file>
@@ -131,9 +131,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1136,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D212DAE-41B9-48BB-90C6-C7B81A14720A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,56 +1150,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" t="s">
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>80</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1228,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44DE501-A4F1-4E55-9F83-CC17A103164F}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,40 +1244,40 @@
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
agrandissement taille carte model + vue non voulu
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\first_flutter_app\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF35D9D-AE73-494D-B85D-D372A4D2604E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A086F0B4-20C8-47B2-B1C5-DB12ED8DC0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6645" yWindow="3585" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="21">
   <si>
     <t>HERBE</t>
   </si>
@@ -415,15 +415,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -469,8 +469,38 @@
       <c r="O1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" t="s">
+        <v>2</v>
+      </c>
+      <c r="W1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -514,10 +544,40 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -561,10 +621,40 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -608,10 +698,40 @@
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -655,10 +775,40 @@
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1</v>
+      </c>
+      <c r="S5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
+        <v>1</v>
+      </c>
+      <c r="V5" t="s">
+        <v>1</v>
+      </c>
+      <c r="W5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -702,10 +852,40 @@
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
+        <v>1</v>
+      </c>
+      <c r="T6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U6" t="s">
+        <v>1</v>
+      </c>
+      <c r="V6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -749,10 +929,40 @@
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T7" t="s">
+        <v>1</v>
+      </c>
+      <c r="U7" t="s">
+        <v>1</v>
+      </c>
+      <c r="V7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W7" t="s">
+        <v>1</v>
+      </c>
+      <c r="X7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -796,10 +1006,40 @@
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" t="s">
+        <v>1</v>
+      </c>
+      <c r="V8" t="s">
+        <v>1</v>
+      </c>
+      <c r="W8" t="s">
+        <v>1</v>
+      </c>
+      <c r="X8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -843,10 +1083,40 @@
         <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
+        <v>1</v>
+      </c>
+      <c r="T9" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9" t="s">
+        <v>1</v>
+      </c>
+      <c r="V9" t="s">
+        <v>1</v>
+      </c>
+      <c r="W9" t="s">
+        <v>1</v>
+      </c>
+      <c r="X9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -890,10 +1160,40 @@
         <v>1</v>
       </c>
       <c r="O10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" t="s">
+        <v>1</v>
+      </c>
+      <c r="T10" t="s">
+        <v>1</v>
+      </c>
+      <c r="U10" t="s">
+        <v>1</v>
+      </c>
+      <c r="V10" t="s">
+        <v>1</v>
+      </c>
+      <c r="W10" t="s">
+        <v>1</v>
+      </c>
+      <c r="X10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -937,10 +1237,40 @@
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" t="s">
+        <v>1</v>
+      </c>
+      <c r="S11" t="s">
+        <v>1</v>
+      </c>
+      <c r="T11" t="s">
+        <v>1</v>
+      </c>
+      <c r="U11" t="s">
+        <v>1</v>
+      </c>
+      <c r="V11" t="s">
+        <v>1</v>
+      </c>
+      <c r="W11" t="s">
+        <v>1</v>
+      </c>
+      <c r="X11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -984,10 +1314,40 @@
         <v>1</v>
       </c>
       <c r="O12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
+        <v>1</v>
+      </c>
+      <c r="S12" t="s">
+        <v>1</v>
+      </c>
+      <c r="T12" t="s">
+        <v>1</v>
+      </c>
+      <c r="U12" t="s">
+        <v>1</v>
+      </c>
+      <c r="V12" t="s">
+        <v>1</v>
+      </c>
+      <c r="W12" t="s">
+        <v>1</v>
+      </c>
+      <c r="X12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1031,10 +1391,40 @@
         <v>1</v>
       </c>
       <c r="O13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
+        <v>1</v>
+      </c>
+      <c r="S13" t="s">
+        <v>1</v>
+      </c>
+      <c r="T13" t="s">
+        <v>1</v>
+      </c>
+      <c r="U13" t="s">
+        <v>1</v>
+      </c>
+      <c r="V13" t="s">
+        <v>1</v>
+      </c>
+      <c r="W13" t="s">
+        <v>1</v>
+      </c>
+      <c r="X13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1051,80 +1441,910 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" t="s">
         <v>1</v>
       </c>
       <c r="O14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S14" t="s">
+        <v>1</v>
+      </c>
+      <c r="T14" t="s">
+        <v>1</v>
+      </c>
+      <c r="U14" t="s">
+        <v>1</v>
+      </c>
+      <c r="V14" t="s">
+        <v>1</v>
+      </c>
+      <c r="W14" t="s">
+        <v>1</v>
+      </c>
+      <c r="X14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O15" t="s">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>1</v>
+      </c>
+      <c r="S15" t="s">
+        <v>1</v>
+      </c>
+      <c r="T15" t="s">
+        <v>1</v>
+      </c>
+      <c r="U15" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" t="s">
+        <v>1</v>
+      </c>
+      <c r="W15" t="s">
+        <v>1</v>
+      </c>
+      <c r="X15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O16" t="s">
+        <v>1</v>
+      </c>
+      <c r="P16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
+        <v>1</v>
+      </c>
+      <c r="S16" t="s">
+        <v>1</v>
+      </c>
+      <c r="T16" t="s">
+        <v>1</v>
+      </c>
+      <c r="U16" t="s">
+        <v>1</v>
+      </c>
+      <c r="V16" t="s">
+        <v>1</v>
+      </c>
+      <c r="W16" t="s">
+        <v>1</v>
+      </c>
+      <c r="X16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" t="s">
+        <v>1</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" t="s">
+        <v>1</v>
+      </c>
+      <c r="T17" t="s">
+        <v>1</v>
+      </c>
+      <c r="U17" t="s">
+        <v>1</v>
+      </c>
+      <c r="V17" t="s">
+        <v>1</v>
+      </c>
+      <c r="W17" t="s">
+        <v>1</v>
+      </c>
+      <c r="X17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O18" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>1</v>
+      </c>
+      <c r="S18" t="s">
+        <v>1</v>
+      </c>
+      <c r="T18" t="s">
+        <v>1</v>
+      </c>
+      <c r="U18" t="s">
+        <v>1</v>
+      </c>
+      <c r="V18" t="s">
+        <v>1</v>
+      </c>
+      <c r="W18" t="s">
+        <v>1</v>
+      </c>
+      <c r="X18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1</v>
+      </c>
+      <c r="O19" t="s">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
+        <v>1</v>
+      </c>
+      <c r="S19" t="s">
+        <v>1</v>
+      </c>
+      <c r="T19" t="s">
+        <v>1</v>
+      </c>
+      <c r="U19" t="s">
+        <v>1</v>
+      </c>
+      <c r="V19" t="s">
+        <v>1</v>
+      </c>
+      <c r="W19" t="s">
+        <v>1</v>
+      </c>
+      <c r="X19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" t="s">
+        <v>1</v>
+      </c>
+      <c r="M20" t="s">
+        <v>1</v>
+      </c>
+      <c r="N20" t="s">
+        <v>1</v>
+      </c>
+      <c r="O20" t="s">
+        <v>1</v>
+      </c>
+      <c r="P20" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>1</v>
+      </c>
+      <c r="R20" t="s">
+        <v>1</v>
+      </c>
+      <c r="S20" t="s">
+        <v>1</v>
+      </c>
+      <c r="T20" t="s">
+        <v>1</v>
+      </c>
+      <c r="U20" t="s">
+        <v>1</v>
+      </c>
+      <c r="V20" t="s">
+        <v>1</v>
+      </c>
+      <c r="W20" t="s">
+        <v>1</v>
+      </c>
+      <c r="X20" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" t="s">
+        <v>1</v>
+      </c>
+      <c r="M21" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
+        <v>1</v>
+      </c>
+      <c r="O21" t="s">
+        <v>1</v>
+      </c>
+      <c r="P21" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" t="s">
+        <v>1</v>
+      </c>
+      <c r="S21" t="s">
+        <v>1</v>
+      </c>
+      <c r="T21" t="s">
+        <v>1</v>
+      </c>
+      <c r="U21" t="s">
+        <v>1</v>
+      </c>
+      <c r="V21" t="s">
+        <v>1</v>
+      </c>
+      <c r="W21" t="s">
+        <v>1</v>
+      </c>
+      <c r="X21" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" t="s">
+        <v>1</v>
+      </c>
+      <c r="N22" t="s">
+        <v>1</v>
+      </c>
+      <c r="O22" t="s">
+        <v>1</v>
+      </c>
+      <c r="P22" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" t="s">
+        <v>1</v>
+      </c>
+      <c r="S22" t="s">
+        <v>1</v>
+      </c>
+      <c r="T22" t="s">
+        <v>1</v>
+      </c>
+      <c r="U22" t="s">
+        <v>1</v>
+      </c>
+      <c r="V22" t="s">
+        <v>1</v>
+      </c>
+      <c r="W22" t="s">
+        <v>1</v>
+      </c>
+      <c r="X22" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
+        <v>1</v>
+      </c>
+      <c r="M23" t="s">
+        <v>1</v>
+      </c>
+      <c r="N23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" t="s">
+        <v>1</v>
+      </c>
+      <c r="S23" t="s">
+        <v>1</v>
+      </c>
+      <c r="T23" t="s">
+        <v>1</v>
+      </c>
+      <c r="U23" t="s">
+        <v>1</v>
+      </c>
+      <c r="V23" t="s">
+        <v>1</v>
+      </c>
+      <c r="W23" t="s">
+        <v>1</v>
+      </c>
+      <c r="X23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>1</v>
+      </c>
+      <c r="L24" t="s">
+        <v>1</v>
+      </c>
+      <c r="M24" t="s">
+        <v>1</v>
+      </c>
+      <c r="N24" t="s">
+        <v>1</v>
+      </c>
+      <c r="O24" t="s">
+        <v>1</v>
+      </c>
+      <c r="P24" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>1</v>
+      </c>
+      <c r="R24" t="s">
+        <v>1</v>
+      </c>
+      <c r="S24" t="s">
+        <v>1</v>
+      </c>
+      <c r="T24" t="s">
+        <v>1</v>
+      </c>
+      <c r="U24" t="s">
+        <v>1</v>
+      </c>
+      <c r="V24" t="s">
+        <v>1</v>
+      </c>
+      <c r="W24" t="s">
+        <v>1</v>
+      </c>
+      <c r="X24" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25" t="s">
+        <v>2</v>
+      </c>
+      <c r="L25" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" t="s">
+        <v>2</v>
+      </c>
+      <c r="N25" t="s">
+        <v>2</v>
+      </c>
+      <c r="O25" t="s">
+        <v>2</v>
+      </c>
+      <c r="P25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>2</v>
+      </c>
+      <c r="R25" t="s">
+        <v>2</v>
+      </c>
+      <c r="S25" t="s">
+        <v>2</v>
+      </c>
+      <c r="T25" t="s">
+        <v>2</v>
+      </c>
+      <c r="U25" t="s">
+        <v>2</v>
+      </c>
+      <c r="V25" t="s">
+        <v>2</v>
+      </c>
+      <c r="W25" t="s">
+        <v>2</v>
+      </c>
+      <c r="X25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y25" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1137,7 +2357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D212DAE-41B9-48BB-90C6-C7B81A14720A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
donnes par exel et taille model implicite
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\first_flutter_app\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A086F0B4-20C8-47B2-B1C5-DB12ED8DC0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F210EBE-E4D8-416A-91A1-E46D61669D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
-    <sheet name="element_terrain" sheetId="2" r:id="rId2"/>
-    <sheet name="pokemon" sheetId="3" r:id="rId3"/>
+    <sheet name="donnees" sheetId="4" r:id="rId2"/>
+    <sheet name="element_terrain" sheetId="2" r:id="rId3"/>
+    <sheet name="pokemon" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="24">
   <si>
     <t>HERBE</t>
   </si>
@@ -90,6 +91,15 @@
   </si>
   <si>
     <t>33.3</t>
+  </si>
+  <si>
+    <t>taille carte vue</t>
+  </si>
+  <si>
+    <t>x spawn hero</t>
+  </si>
+  <si>
+    <t>y spawn hero</t>
   </si>
 </sst>
 </file>
@@ -417,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25:Y25"/>
     </sheetView>
   </sheetViews>
@@ -2354,6 +2364,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2183D8-49B1-4F0B-B007-814726321D84}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D212DAE-41B9-48BB-90C6-C7B81A14720A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -2445,7 +2497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44DE501-A4F1-4E55-9F83-CC17A103164F}">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>

<commit_message>
on peut faire la map rectangle que l'on veut
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\first_flutter_app\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F210EBE-E4D8-416A-91A1-E46D61669D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081924BA-B2F3-452A-95B3-FDD0CAFD3C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="24">
   <si>
     <t>HERBE</t>
   </si>
@@ -425,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:Y25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -509,8 +509,11 @@
       <c r="Y1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -586,8 +589,11 @@
       <c r="Y2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -661,10 +667,13 @@
         <v>1</v>
       </c>
       <c r="Y3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -740,8 +749,11 @@
       <c r="Y4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -817,8 +829,11 @@
       <c r="Y5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -894,8 +909,11 @@
       <c r="Y6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -971,8 +989,11 @@
       <c r="Y7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1048,8 +1069,11 @@
       <c r="Y8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1125,8 +1149,11 @@
       <c r="Y9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1202,8 +1229,11 @@
       <c r="Y10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1279,8 +1309,11 @@
       <c r="Y11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1356,1005 +1389,87 @@
       <c r="Y12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
-        <v>1</v>
-      </c>
-      <c r="K14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L14" t="s">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>1</v>
-      </c>
-      <c r="N14" t="s">
-        <v>1</v>
-      </c>
-      <c r="O14" t="s">
-        <v>1</v>
-      </c>
-      <c r="P14" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>1</v>
-      </c>
-      <c r="R14" t="s">
-        <v>1</v>
-      </c>
-      <c r="S14" t="s">
-        <v>1</v>
-      </c>
-      <c r="T14" t="s">
-        <v>1</v>
-      </c>
-      <c r="U14" t="s">
-        <v>1</v>
-      </c>
-      <c r="V14" t="s">
-        <v>1</v>
-      </c>
-      <c r="W14" t="s">
-        <v>1</v>
-      </c>
-      <c r="X14" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>1</v>
-      </c>
-      <c r="K15" t="s">
-        <v>1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M15" t="s">
-        <v>1</v>
-      </c>
-      <c r="N15" t="s">
-        <v>1</v>
-      </c>
-      <c r="O15" t="s">
-        <v>1</v>
-      </c>
-      <c r="P15" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>1</v>
-      </c>
-      <c r="R15" t="s">
-        <v>1</v>
-      </c>
-      <c r="S15" t="s">
-        <v>1</v>
-      </c>
-      <c r="T15" t="s">
-        <v>1</v>
-      </c>
-      <c r="U15" t="s">
-        <v>1</v>
-      </c>
-      <c r="V15" t="s">
-        <v>1</v>
-      </c>
-      <c r="W15" t="s">
-        <v>1</v>
-      </c>
-      <c r="X15" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
-        <v>1</v>
-      </c>
-      <c r="K16" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M16" t="s">
-        <v>1</v>
-      </c>
-      <c r="N16" t="s">
-        <v>1</v>
-      </c>
-      <c r="O16" t="s">
-        <v>1</v>
-      </c>
-      <c r="P16" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>1</v>
-      </c>
-      <c r="R16" t="s">
-        <v>1</v>
-      </c>
-      <c r="S16" t="s">
-        <v>1</v>
-      </c>
-      <c r="T16" t="s">
-        <v>1</v>
-      </c>
-      <c r="U16" t="s">
-        <v>1</v>
-      </c>
-      <c r="V16" t="s">
-        <v>1</v>
-      </c>
-      <c r="W16" t="s">
-        <v>1</v>
-      </c>
-      <c r="X16" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" t="s">
-        <v>1</v>
-      </c>
-      <c r="L17" t="s">
-        <v>1</v>
-      </c>
-      <c r="M17" t="s">
-        <v>1</v>
-      </c>
-      <c r="N17" t="s">
-        <v>1</v>
-      </c>
-      <c r="O17" t="s">
-        <v>1</v>
-      </c>
-      <c r="P17" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>1</v>
-      </c>
-      <c r="R17" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" t="s">
-        <v>1</v>
-      </c>
-      <c r="T17" t="s">
-        <v>1</v>
-      </c>
-      <c r="U17" t="s">
-        <v>1</v>
-      </c>
-      <c r="V17" t="s">
-        <v>1</v>
-      </c>
-      <c r="W17" t="s">
-        <v>1</v>
-      </c>
-      <c r="X17" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" t="s">
-        <v>1</v>
-      </c>
-      <c r="M18" t="s">
-        <v>1</v>
-      </c>
-      <c r="N18" t="s">
-        <v>1</v>
-      </c>
-      <c r="O18" t="s">
-        <v>1</v>
-      </c>
-      <c r="P18" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>1</v>
-      </c>
-      <c r="R18" t="s">
-        <v>1</v>
-      </c>
-      <c r="S18" t="s">
-        <v>1</v>
-      </c>
-      <c r="T18" t="s">
-        <v>1</v>
-      </c>
-      <c r="U18" t="s">
-        <v>1</v>
-      </c>
-      <c r="V18" t="s">
-        <v>1</v>
-      </c>
-      <c r="W18" t="s">
-        <v>1</v>
-      </c>
-      <c r="X18" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19" t="s">
-        <v>1</v>
-      </c>
-      <c r="K19" t="s">
-        <v>1</v>
-      </c>
-      <c r="L19" t="s">
-        <v>1</v>
-      </c>
-      <c r="M19" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" t="s">
-        <v>1</v>
-      </c>
-      <c r="O19" t="s">
-        <v>1</v>
-      </c>
-      <c r="P19" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>1</v>
-      </c>
-      <c r="R19" t="s">
-        <v>1</v>
-      </c>
-      <c r="S19" t="s">
-        <v>1</v>
-      </c>
-      <c r="T19" t="s">
-        <v>1</v>
-      </c>
-      <c r="U19" t="s">
-        <v>1</v>
-      </c>
-      <c r="V19" t="s">
-        <v>1</v>
-      </c>
-      <c r="W19" t="s">
-        <v>1</v>
-      </c>
-      <c r="X19" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20" t="s">
-        <v>1</v>
-      </c>
-      <c r="I20" t="s">
-        <v>1</v>
-      </c>
-      <c r="J20" t="s">
-        <v>1</v>
-      </c>
-      <c r="K20" t="s">
-        <v>1</v>
-      </c>
-      <c r="L20" t="s">
-        <v>1</v>
-      </c>
-      <c r="M20" t="s">
-        <v>1</v>
-      </c>
-      <c r="N20" t="s">
-        <v>1</v>
-      </c>
-      <c r="O20" t="s">
-        <v>1</v>
-      </c>
-      <c r="P20" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>1</v>
-      </c>
-      <c r="R20" t="s">
-        <v>1</v>
-      </c>
-      <c r="S20" t="s">
-        <v>1</v>
-      </c>
-      <c r="T20" t="s">
-        <v>1</v>
-      </c>
-      <c r="U20" t="s">
-        <v>1</v>
-      </c>
-      <c r="V20" t="s">
-        <v>1</v>
-      </c>
-      <c r="W20" t="s">
-        <v>1</v>
-      </c>
-      <c r="X20" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" t="s">
-        <v>1</v>
-      </c>
-      <c r="J21" t="s">
-        <v>1</v>
-      </c>
-      <c r="K21" t="s">
-        <v>1</v>
-      </c>
-      <c r="L21" t="s">
-        <v>1</v>
-      </c>
-      <c r="M21" t="s">
-        <v>1</v>
-      </c>
-      <c r="N21" t="s">
-        <v>1</v>
-      </c>
-      <c r="O21" t="s">
-        <v>1</v>
-      </c>
-      <c r="P21" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>1</v>
-      </c>
-      <c r="R21" t="s">
-        <v>1</v>
-      </c>
-      <c r="S21" t="s">
-        <v>1</v>
-      </c>
-      <c r="T21" t="s">
-        <v>1</v>
-      </c>
-      <c r="U21" t="s">
-        <v>1</v>
-      </c>
-      <c r="V21" t="s">
-        <v>1</v>
-      </c>
-      <c r="W21" t="s">
-        <v>1</v>
-      </c>
-      <c r="X21" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
-        <v>1</v>
-      </c>
-      <c r="I22" t="s">
-        <v>1</v>
-      </c>
-      <c r="J22" t="s">
-        <v>1</v>
-      </c>
-      <c r="K22" t="s">
-        <v>1</v>
-      </c>
-      <c r="L22" t="s">
-        <v>1</v>
-      </c>
-      <c r="M22" t="s">
-        <v>1</v>
-      </c>
-      <c r="N22" t="s">
-        <v>1</v>
-      </c>
-      <c r="O22" t="s">
-        <v>1</v>
-      </c>
-      <c r="P22" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>1</v>
-      </c>
-      <c r="R22" t="s">
-        <v>1</v>
-      </c>
-      <c r="S22" t="s">
-        <v>1</v>
-      </c>
-      <c r="T22" t="s">
-        <v>1</v>
-      </c>
-      <c r="U22" t="s">
-        <v>1</v>
-      </c>
-      <c r="V22" t="s">
-        <v>1</v>
-      </c>
-      <c r="W22" t="s">
-        <v>1</v>
-      </c>
-      <c r="X22" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" t="s">
-        <v>1</v>
-      </c>
-      <c r="J23" t="s">
-        <v>1</v>
-      </c>
-      <c r="K23" t="s">
-        <v>1</v>
-      </c>
-      <c r="L23" t="s">
-        <v>1</v>
-      </c>
-      <c r="M23" t="s">
-        <v>1</v>
-      </c>
-      <c r="N23" t="s">
-        <v>1</v>
-      </c>
-      <c r="O23" t="s">
-        <v>1</v>
-      </c>
-      <c r="P23" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>1</v>
-      </c>
-      <c r="R23" t="s">
-        <v>1</v>
-      </c>
-      <c r="S23" t="s">
-        <v>1</v>
-      </c>
-      <c r="T23" t="s">
-        <v>1</v>
-      </c>
-      <c r="U23" t="s">
-        <v>1</v>
-      </c>
-      <c r="V23" t="s">
-        <v>1</v>
-      </c>
-      <c r="W23" t="s">
-        <v>1</v>
-      </c>
-      <c r="X23" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" t="s">
-        <v>1</v>
-      </c>
-      <c r="I24" t="s">
-        <v>1</v>
-      </c>
-      <c r="J24" t="s">
-        <v>1</v>
-      </c>
-      <c r="K24" t="s">
-        <v>1</v>
-      </c>
-      <c r="L24" t="s">
-        <v>1</v>
-      </c>
-      <c r="M24" t="s">
-        <v>1</v>
-      </c>
-      <c r="N24" t="s">
-        <v>1</v>
-      </c>
-      <c r="O24" t="s">
-        <v>1</v>
-      </c>
-      <c r="P24" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>1</v>
-      </c>
-      <c r="R24" t="s">
-        <v>1</v>
-      </c>
-      <c r="S24" t="s">
-        <v>1</v>
-      </c>
-      <c r="T24" t="s">
-        <v>1</v>
-      </c>
-      <c r="U24" t="s">
-        <v>1</v>
-      </c>
-      <c r="V24" t="s">
-        <v>1</v>
-      </c>
-      <c r="W24" t="s">
-        <v>1</v>
-      </c>
-      <c r="X24" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" t="s">
-        <v>2</v>
-      </c>
-      <c r="G25" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25" t="s">
-        <v>2</v>
-      </c>
-      <c r="I25" t="s">
-        <v>2</v>
-      </c>
-      <c r="J25" t="s">
-        <v>2</v>
-      </c>
-      <c r="K25" t="s">
-        <v>2</v>
-      </c>
-      <c r="L25" t="s">
-        <v>2</v>
-      </c>
-      <c r="M25" t="s">
-        <v>2</v>
-      </c>
-      <c r="N25" t="s">
-        <v>2</v>
-      </c>
-      <c r="O25" t="s">
-        <v>2</v>
-      </c>
-      <c r="P25" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>2</v>
-      </c>
-      <c r="R25" t="s">
-        <v>2</v>
-      </c>
-      <c r="S25" t="s">
-        <v>2</v>
-      </c>
-      <c r="T25" t="s">
-        <v>2</v>
-      </c>
-      <c r="U25" t="s">
-        <v>2</v>
-      </c>
-      <c r="V25" t="s">
-        <v>2</v>
-      </c>
-      <c r="W25" t="s">
-        <v>2</v>
-      </c>
-      <c r="X25" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y25" t="s">
+      <c r="Z13" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2367,7 +1482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2183D8-49B1-4F0B-B007-814726321D84}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
le modele de combat focntionne
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\first_flutter_app\assets\for_alex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\pacomon\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081924BA-B2F3-452A-95B3-FDD0CAFD3C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7F4F0D-9C75-4745-94EA-22510CF64A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="12135" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="27">
   <si>
     <t>HERBE</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>y spawn hero</t>
+  </si>
+  <si>
+    <t>atk</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>pvMax</t>
   </si>
 </sst>
 </file>
@@ -427,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
@@ -1614,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44DE501-A4F1-4E55-9F83-CC17A103164F}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,7 +1636,7 @@
     <col min="3" max="3" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1637,8 +1646,17 @@
       <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1648,8 +1666,17 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1659,11 +1686,20 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hautes herbes avec differents pokemons
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\pacomon\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7F4F0D-9C75-4745-94EA-22510CF64A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F869D473-79B8-48C8-9F37-25BF4AC89F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="12135" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="34">
   <si>
     <t>HERBE</t>
   </si>
@@ -42,9 +42,6 @@
     <t>element (ex: HERBE)</t>
   </si>
   <si>
-    <t>chemin image (ex: /assets/une_image.png)</t>
-  </si>
-  <si>
     <t xml:space="preserve">traversable (ex: OUI) (ex: NON) </t>
   </si>
   <si>
@@ -54,61 +51,85 @@
     <t>NON</t>
   </si>
   <si>
+    <t>% proba trouver pokemon (ex: 60)</t>
+  </si>
+  <si>
+    <t>Nom pokemon (ex: Pikatchu)</t>
+  </si>
+  <si>
+    <t>Pikachu</t>
+  </si>
+  <si>
+    <t>Mewtwo</t>
+  </si>
+  <si>
+    <t>rareté (%)</t>
+  </si>
+  <si>
+    <t>chemin image pkmn (ex: /assets … )</t>
+  </si>
+  <si>
+    <t>66.7</t>
+  </si>
+  <si>
+    <t>33.3</t>
+  </si>
+  <si>
+    <t>taille carte vue</t>
+  </si>
+  <si>
+    <t>x spawn hero</t>
+  </si>
+  <si>
+    <t>y spawn hero</t>
+  </si>
+  <si>
+    <t>atk</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>pvMax</t>
+  </si>
+  <si>
+    <t>Categorie</t>
+  </si>
+  <si>
+    <t>DEBUT</t>
+  </si>
+  <si>
     <t>assets/for_alex/herbe.png</t>
   </si>
   <si>
+    <t>chemin image (ex: assets/une_image.png)</t>
+  </si>
+  <si>
     <t>assets/for_alex/sol.png</t>
   </si>
   <si>
     <t>assets/for_alex/rocher.png</t>
   </si>
   <si>
-    <t>% proba trouver pokemon (ex: 60)</t>
-  </si>
-  <si>
-    <t>Nom pokemon (ex: Pikatchu)</t>
-  </si>
-  <si>
-    <t>Pikachu</t>
-  </si>
-  <si>
-    <t>Mewtwo</t>
-  </si>
-  <si>
-    <t>rareté (%)</t>
-  </si>
-  <si>
     <t>assets/for_alex/pikachu.png</t>
   </si>
   <si>
     <t>assets/for_alex/mewtwo.png</t>
   </si>
   <si>
-    <t>chemin image pkmn (ex: /assets … )</t>
-  </si>
-  <si>
-    <t>66.7</t>
-  </si>
-  <si>
-    <t>33.3</t>
-  </si>
-  <si>
-    <t>taille carte vue</t>
-  </si>
-  <si>
-    <t>x spawn hero</t>
-  </si>
-  <si>
-    <t>y spawn hero</t>
-  </si>
-  <si>
-    <t>atk</t>
-  </si>
-  <si>
-    <t>def</t>
-  </si>
-  <si>
-    <t>pvMax</t>
+    <t>HAUTE_HERBE</t>
+  </si>
+  <si>
+    <t>HARD</t>
+  </si>
+  <si>
+    <t>Dracofeu</t>
+  </si>
+  <si>
+    <t>assets/for_alex/dracofeu.png</t>
+  </si>
+  <si>
+    <t>100.0</t>
   </si>
 </sst>
 </file>
@@ -436,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +691,7 @@
         <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="X3" t="s">
         <v>1</v>
@@ -1502,7 +1523,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B1">
         <v>15</v>
@@ -1510,7 +1531,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -1518,7 +1539,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -1531,89 +1552,115 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D212DAE-41B9-48BB-90C6-C7B81A14720A}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.140625" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
   </sheetData>
@@ -1623,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44DE501-A4F1-4E55-9F83-CC17A103164F}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,70 +1683,99 @@
     <col min="3" max="3" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
       <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3">
         <v>20</v>
       </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
+      <c r="F3">
         <v>100</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4">
+        <v>200</v>
+      </c>
+      <c r="F4">
+        <v>200</v>
+      </c>
+      <c r="G4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout de la selection de stat perso
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\pacomon\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F869D473-79B8-48C8-9F37-25BF4AC89F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C46587E-8317-4180-A389-D49CCB19E85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="39">
   <si>
     <t>HERBE</t>
   </si>
@@ -130,6 +130,21 @@
   </si>
   <si>
     <t>100.0</t>
+  </si>
+  <si>
+    <t>atk hero</t>
+  </si>
+  <si>
+    <t>def hero</t>
+  </si>
+  <si>
+    <t>pv hero</t>
+  </si>
+  <si>
+    <t>% augmentation stats par level</t>
+  </si>
+  <si>
+    <t>10.0</t>
   </si>
 </sst>
 </file>
@@ -1510,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2183D8-49B1-4F0B-B007-814726321D84}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,6 +1558,38 @@
       </c>
       <c r="B3">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1672,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44DE501-A4F1-4E55-9F83-CC17A103164F}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ajout de la vitesse
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\pacomon\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB90F25B-C1E3-4FB5-B067-9848327851BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C35C1E-53BD-4191-A331-3A6A6F0F7BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4905" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="41">
   <si>
     <t>HERBE</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>exp</t>
+  </si>
+  <si>
+    <t>vitesse</t>
   </si>
 </sst>
 </file>
@@ -1530,7 +1533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2183D8-49B1-4F0B-B007-814726321D84}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1720,10 +1723,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44DE501-A4F1-4E55-9F83-CC17A103164F}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,7 +1736,7 @@
     <col min="3" max="3" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1756,10 +1759,13 @@
         <v>20</v>
       </c>
       <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1770,7 +1776,7 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1784,8 +1790,11 @@
       <c r="H2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1796,7 +1805,7 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>20</v>
@@ -1808,10 +1817,13 @@
         <v>200</v>
       </c>
       <c r="H3">
+        <v>50</v>
+      </c>
+      <c r="I3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -1834,10 +1846,13 @@
         <v>2000</v>
       </c>
       <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout des centres de guerison 2
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\pacomon\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C35C1E-53BD-4191-A331-3A6A6F0F7BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4AB691-FC09-4163-A69B-4AE4A0F78FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4905" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5685" yWindow="4020" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="46">
   <si>
     <t>HERBE</t>
   </si>
@@ -151,6 +151,21 @@
   </si>
   <si>
     <t>vitesse</t>
+  </si>
+  <si>
+    <t>intercation</t>
+  </si>
+  <si>
+    <t>RIEN</t>
+  </si>
+  <si>
+    <t>CENTRE_PACOMON</t>
+  </si>
+  <si>
+    <t>CENTRE</t>
+  </si>
+  <si>
+    <t>assets/for_alex/centre_guerison.png</t>
   </si>
 </sst>
 </file>
@@ -478,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="O5" t="s">
         <v>1</v>
@@ -1605,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D212DAE-41B9-48BB-90C6-C7B81A14720A}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,7 +1634,7 @@
     <col min="4" max="4" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1635,8 +1650,11 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1652,8 +1670,11 @@
       <c r="E2">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1669,8 +1690,11 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1686,8 +1710,11 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -1703,17 +1730,37 @@
       <c r="E5">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
   </sheetData>
@@ -1725,7 +1772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44DE501-A4F1-4E55-9F83-CC17A103164F}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ajout de la stat de vitesse dans les stats vue
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\pacomon\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4AB691-FC09-4163-A69B-4AE4A0F78FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263A9107-CD8D-4049-A4B5-4986F3137BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5685" yWindow="4020" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5685" yWindow="4020" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="51">
   <si>
     <t>HERBE</t>
   </si>
@@ -166,16 +166,37 @@
   </si>
   <si>
     <t>assets/for_alex/centre_guerison.png</t>
+  </si>
+  <si>
+    <t>vit hero</t>
+  </si>
+  <si>
+    <t>pp attaque  1</t>
+  </si>
+  <si>
+    <t>pp attaque  2</t>
+  </si>
+  <si>
+    <t>pp attaque  3</t>
+  </si>
+  <si>
+    <t>pp attaque  4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -493,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -1546,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2183D8-49B1-4F0B-B007-814726321D84}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,13 +1628,54 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>38</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
ajout de la maitrise
</commit_message>
<xml_diff>
--- a/assets/for_alex/database_run.xlsx
+++ b/assets/for_alex/database_run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STOCKAGE\code\vscode\projects\flutter\pacomon\assets\for_alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263A9107-CD8D-4049-A4B5-4986F3137BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523419D5-30BE-41C7-B6F8-67EBB744F87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5685" yWindow="4020" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carte" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="55">
   <si>
     <t>HERBE</t>
   </si>
@@ -132,21 +132,6 @@
     <t>100.0</t>
   </si>
   <si>
-    <t>atk hero</t>
-  </si>
-  <si>
-    <t>def hero</t>
-  </si>
-  <si>
-    <t>pv hero</t>
-  </si>
-  <si>
-    <t>% augmentation stats par level</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
     <t>exp</t>
   </si>
   <si>
@@ -168,19 +153,46 @@
     <t>assets/for_alex/centre_guerison.png</t>
   </si>
   <si>
-    <t>vit hero</t>
-  </si>
-  <si>
-    <t>pp attaque  1</t>
-  </si>
-  <si>
-    <t>pp attaque  2</t>
-  </si>
-  <si>
-    <t>pp attaque  3</t>
-  </si>
-  <si>
-    <t>pp attaque  4</t>
+    <t>atk base  hero</t>
+  </si>
+  <si>
+    <t>def base hero</t>
+  </si>
+  <si>
+    <t>pv base hero</t>
+  </si>
+  <si>
+    <t>vit base hero</t>
+  </si>
+  <si>
+    <t>pp base attaque  1</t>
+  </si>
+  <si>
+    <t>pp base attaque  2</t>
+  </si>
+  <si>
+    <t>pp base attaque  3</t>
+  </si>
+  <si>
+    <t>pp base attaque  4</t>
+  </si>
+  <si>
+    <t>point maitrise gagné par niv</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + atk par pt maitrise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + def par pt maitrise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + vit par pt maitrise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + pv par pt maitrise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + pp par pt maitrise</t>
   </si>
 </sst>
 </file>
@@ -881,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="O5" t="s">
         <v>1</v>
@@ -1567,10 +1579,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2183D8-49B1-4F0B-B007-814726321D84}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,7 +1616,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>10000</v>
@@ -1612,7 +1624,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1620,7 +1632,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B6">
         <v>777</v>
@@ -1628,7 +1640,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -1636,42 +1648,82 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>50</v>
       </c>
-      <c r="B12">
-        <v>8</v>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1713,7 +1765,7 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1733,7 +1785,7 @@
         <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1753,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1773,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1793,15 +1845,15 @@
         <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -1813,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1868,10 +1920,10 @@
         <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>